<commit_message>
Model - added development testing RunType = 2.
Ruleset - changed Havasu Rule Curve Rule to reflect this.
</commit_message>
<xml_diff>
--- a/Input Data/DevTesting/DevTesting_IC.wet.xlsx
+++ b/Input Data/DevTesting/DevTesting_IC.wet.xlsx
@@ -505,7 +505,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="N2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="V4" sqref="V4"/>
+      <selection pane="bottomRight" activeCell="V21" sqref="V21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1935,7 +1935,7 @@
         <v>951252.89</v>
       </c>
       <c r="T21" s="6">
-        <v>727063.99999834399</v>
+        <v>4557217</v>
       </c>
       <c r="U21">
         <v>1644196</v>

</xml_diff>